<commit_message>
WIP multiple sub objects
</commit_message>
<xml_diff>
--- a/parser_output/webapp_json.xlsx
+++ b/parser_output/webapp_json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quan\Documents\project_2023\parser\parser_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C029244E-96A3-4C6D-9DEA-0193587B636F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E521EE57-A7F2-479A-85FC-E1B4C4308519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="772">
   <si>
     <t>Area</t>
   </si>
@@ -967,7 +967,10 @@
     <t>Aggiungi nuovo macinacaffè</t>
   </si>
   <si>
-    <t>addGrinderContent:Inseriscinumerodimatricola</t>
+    <t>addGrinderContent</t>
+  </si>
+  <si>
+    <t>Inserisci numero di matricola:</t>
   </si>
   <si>
     <t>deleteGrinderTitle</t>
@@ -1297,7 +1300,10 @@
     <t>Chiudi la Rappresentazione</t>
   </si>
   <si>
-    <t>impersonating:Impersonarel'utente</t>
+    <t>impersonating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impersonare l'utente: </t>
   </si>
   <si>
     <t>licenseManagement</t>
@@ -2683,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D411"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4934,6 +4940,12 @@
       <c r="B162" t="s">
         <v>315</v>
       </c>
+      <c r="C162" t="s">
+        <v>316</v>
+      </c>
+      <c r="D162" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
@@ -4968,7 +4980,7 @@
         <v>312</v>
       </c>
       <c r="B165" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C165" t="s">
         <v>286</v>
@@ -4982,13 +4994,13 @@
         <v>312</v>
       </c>
       <c r="B166" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C166" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D166" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,13 +5008,13 @@
         <v>312</v>
       </c>
       <c r="B167" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C167" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D167" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -5010,13 +5022,13 @@
         <v>312</v>
       </c>
       <c r="B168" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C168" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D168" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -5024,13 +5036,13 @@
         <v>312</v>
       </c>
       <c r="B169" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C169" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D169" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5038,13 +5050,13 @@
         <v>312</v>
       </c>
       <c r="B170" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C170" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D170" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5052,13 +5064,13 @@
         <v>312</v>
       </c>
       <c r="B171" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C171" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D171" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5066,13 +5078,13 @@
         <v>312</v>
       </c>
       <c r="B172" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C172" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D172" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5080,13 +5092,13 @@
         <v>312</v>
       </c>
       <c r="B173" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C173" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D173" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,13 +5106,13 @@
         <v>312</v>
       </c>
       <c r="B174" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C174" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D174" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,13 +5120,13 @@
         <v>312</v>
       </c>
       <c r="B175" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C175" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D175" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5122,13 +5134,13 @@
         <v>312</v>
       </c>
       <c r="B176" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C176" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D176" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,13 +5148,13 @@
         <v>312</v>
       </c>
       <c r="B177" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C177" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D177" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -5150,13 +5162,13 @@
         <v>312</v>
       </c>
       <c r="B178" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C178" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D178" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5164,21 +5176,21 @@
         <v>312</v>
       </c>
       <c r="B179" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C179" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D179" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B180" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C180" t="s">
         <v>234</v>
@@ -5189,100 +5201,100 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B181" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C181" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D181" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B182" t="s">
         <v>21</v>
       </c>
       <c r="C182" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D182" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B183" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C183" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D183" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B184" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C184" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D184" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B185" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C185" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D185" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B186" t="s">
         <v>21</v>
       </c>
       <c r="C186" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D186" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B187" t="s">
         <v>207</v>
       </c>
       <c r="C187" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D187" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,10 +5305,10 @@
         <v>21</v>
       </c>
       <c r="C188" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D188" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5304,13 +5316,13 @@
         <v>71</v>
       </c>
       <c r="B189" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C189" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D189" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5318,13 +5330,13 @@
         <v>71</v>
       </c>
       <c r="B190" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C190" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D190" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5332,13 +5344,13 @@
         <v>71</v>
       </c>
       <c r="B191" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C191" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D191" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5346,49 +5358,49 @@
         <v>71</v>
       </c>
       <c r="B192" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C192" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D192" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B193" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C193" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D193" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B194" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C194" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D194" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B195" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C195" t="s">
         <v>60</v>
@@ -5399,21 +5411,21 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B196" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C196" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D196" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B197" t="s">
         <v>298</v>
@@ -5427,189 +5439,189 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B198" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C198" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D198" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B199" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C199" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D199" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B200" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C200" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D200" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B201" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C201" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D201" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B202" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C202" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D202" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B203" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C203" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D203" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B204" t="s">
         <v>21</v>
       </c>
       <c r="C204" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D204" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B205" t="s">
         <v>240</v>
       </c>
       <c r="C205" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D205" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B206" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C206" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D206" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B207" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C207" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D207" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B208" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C208" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D208" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B209" t="s">
         <v>21</v>
       </c>
       <c r="C209" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D209" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B210" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C210" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D210" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B211" t="s">
         <v>238</v>
@@ -5623,35 +5635,35 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B212" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C212" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D212" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B213" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C213" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D213" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B214" t="s">
         <v>303</v>
@@ -5665,10 +5677,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B215" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C215" t="s">
         <v>58</v>
@@ -5679,326 +5691,332 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B216" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C216" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D216" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B217" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C217" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D217" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B218" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C218" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D218" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B219" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C219" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D219" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B220" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C220" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D220" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B221" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C221" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D221" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B222" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C222" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D222" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B223" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C223" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D223" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B224" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C224" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D224" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B225" t="s">
-        <v>425</v>
+        <v>426</v>
+      </c>
+      <c r="C225" t="s">
+        <v>427</v>
+      </c>
+      <c r="D225" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B226" t="s">
         <v>21</v>
       </c>
       <c r="C226" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D226" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B227" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C227" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D227" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B228" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C228" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D228" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B229" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C229" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D229" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B230" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C230" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D230" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B231" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C231" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D231" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B232" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C232" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D232" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B233" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C233" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D233" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B234" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C234" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D234" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B235" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C235" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D235" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B236" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C236" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D236" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B237" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C237" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D237" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B238" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C238" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D238" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B239" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C239" t="s">
         <v>60</v>
@@ -6009,203 +6027,203 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B240" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C240" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D240" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B241" t="s">
         <v>21</v>
       </c>
       <c r="C241" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D241" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B242" t="s">
         <v>207</v>
       </c>
       <c r="C242" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D242" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B243" t="s">
         <v>21</v>
       </c>
       <c r="C243" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D243" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B244" t="s">
         <v>207</v>
       </c>
       <c r="C244" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D244" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B245" t="s">
         <v>21</v>
       </c>
       <c r="C245" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D245" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B246" t="s">
         <v>207</v>
       </c>
       <c r="C246" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D246" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B247" t="s">
         <v>21</v>
       </c>
       <c r="C247" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D247" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B248" t="s">
         <v>207</v>
       </c>
       <c r="C248" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D248" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B249" t="s">
         <v>21</v>
       </c>
       <c r="C249" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D249" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B250" t="s">
         <v>207</v>
       </c>
       <c r="C250" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D250" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C251" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D251" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B252" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C252" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D252" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B253" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C253" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D253" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B254" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C254" t="s">
         <v>286</v>
@@ -6216,10 +6234,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B255" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C255" t="s">
         <v>225</v>
@@ -6230,637 +6248,637 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B256" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C256" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D256" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B257" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C257" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D257" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B258" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C258" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D258" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B259" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C259" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D259" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B260" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C260" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D260" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B261" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C261" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D261" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B262" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C262" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D262" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B263" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C263" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D263" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B264" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C264" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D264" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B265" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C265" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D265" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B266" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C266" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D266" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B267" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C267" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D267" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B268" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C268" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D268" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B269" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C269" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D269" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B270" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C270" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D270" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B271" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C271" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D271" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B272" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C272" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D272" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B273" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C273" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D273" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B274" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C274" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D274" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B275" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C275" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D275" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B276" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C276" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="D276" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B277" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C277" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D277" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B278" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C278" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D278" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B279" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C279" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D279" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B280" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C280" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D280" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B281" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C281" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D281" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B282" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C282" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D282" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B283" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C283" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D283" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B284" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C284" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D284" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B285" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C285" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D285" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B286" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C286" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D286" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B287" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C287" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D287" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B288" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C288" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D288" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B289" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C289" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="D289" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B290" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C290" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D290" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B291" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C291" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D291" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B292" t="s">
         <v>187</v>
       </c>
       <c r="C292" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D292" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B293" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C293" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D293" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B294" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C294" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D294" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B295" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C295" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D295" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B296" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C296" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D296" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B297" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C297" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D297" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B298" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C298" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D298" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B299" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="C299" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D299" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B300" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C300" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D300" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B301" t="s">
         <v>63</v>
@@ -6874,94 +6892,94 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B302" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C302" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D302" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B303" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C303" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="D303" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B304" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C304" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D304" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B305" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C305" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D305" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B306" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C306" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D306" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B307" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C307" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D307" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B308" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C308" t="s">
         <v>105</v>
@@ -6972,91 +6990,91 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B309" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C309" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D309" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B310" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C310" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="D310" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B311" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C311" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D311" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B312" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C312" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D312" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B313" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C313" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="D313" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B314" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C314" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D314" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B315" t="s">
         <v>259</v>
@@ -7070,49 +7088,49 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B316" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C316" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D316" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B317" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C317" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D317" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B318" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C318" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D318" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B319" t="s">
         <v>254</v>
@@ -7126,973 +7144,973 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B320" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C320" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="D320" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B321" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C321" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D321" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B322" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C322" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D322" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B323" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C323" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D323" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B324" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C324" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D324" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B325" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C325" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D325" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B326" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C326" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D326" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B327" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C327" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D327" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B328" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C328" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D328" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B329" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C329" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D329" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B330" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C330" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="D330" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B331" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C331" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="D331" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B332" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C332" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D332" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B333" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="C333" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D333" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B334" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="C334" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D334" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B335" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C335" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D335" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B336" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C336" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D336" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B337" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="C337" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D337" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B338" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C338" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D338" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B339" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="C339" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="D339" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B340" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C340" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D340" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B341" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C341" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D341" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B342" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C342" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D342" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B343" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C343" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D343" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B344" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="C344" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D344" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B345" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="C345" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D345" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B346" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="C346" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D346" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B347" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="C347" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="D347" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B348" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C348" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D348" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B349" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="C349" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="D349" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B350" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C350" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D350" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B351" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="C351" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D351" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B352" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="C352" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="D352" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B353" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C353" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="D353" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B354" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C354" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D354" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B355" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="C355" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="D355" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B356" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C356" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="D356" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B357" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C357" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D357" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B358" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C358" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="D358" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B359" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="C359" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="D359" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B360" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C360" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="D360" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B361" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C361" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D361" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B362" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C362" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D362" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B363" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C363" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D363" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B364" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C364" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D364" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B365" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C365" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D365" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B366" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C366" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="D366" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B367" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C367" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="D367" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B368" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C368" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="D368" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B369" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="C369" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="D369" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B370" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="C370" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="D370" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B371" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C371" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="D371" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B372" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C372" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="D372" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B373" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C373" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="D373" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B374" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C374" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D374" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B375" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C375" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D375" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B376" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C376" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="D376" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B377" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C377" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D377" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B378" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C378" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="D378" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B379" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C379" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D379" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B380" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C380" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="D380" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B381" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C381" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="D381" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B382" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C382" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="D382" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B383" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C383" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="D383" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B384" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C384" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="D384" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B385" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C385" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="D385" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B386" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C386" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D386" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B387" t="s">
         <v>21</v>
       </c>
       <c r="C387" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D387" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B388" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C388" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="D388" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B389" t="s">
         <v>259</v>
@@ -8106,35 +8124,35 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B390" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C390" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D390" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B391" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C391" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D391" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B392" t="s">
         <v>130</v>
@@ -8165,13 +8183,13 @@
         <v>287</v>
       </c>
       <c r="B394" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C394" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D394" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -8179,13 +8197,13 @@
         <v>287</v>
       </c>
       <c r="B395" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C395" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D395" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -8193,13 +8211,13 @@
         <v>287</v>
       </c>
       <c r="B396" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C396" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="D396" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -8207,13 +8225,13 @@
         <v>287</v>
       </c>
       <c r="B397" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="C397" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D397" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
@@ -8221,13 +8239,13 @@
         <v>287</v>
       </c>
       <c r="B398" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="C398" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="D398" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -8235,13 +8253,13 @@
         <v>287</v>
       </c>
       <c r="B399" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C399" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D399" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -8252,10 +8270,10 @@
         <v>303</v>
       </c>
       <c r="C400" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="D400" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
@@ -8263,13 +8281,13 @@
         <v>287</v>
       </c>
       <c r="B401" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C401" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="D401" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -8277,13 +8295,13 @@
         <v>287</v>
       </c>
       <c r="B402" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C402" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="D402" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
@@ -8291,13 +8309,13 @@
         <v>287</v>
       </c>
       <c r="B403" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C403" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="D403" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -8305,13 +8323,13 @@
         <v>287</v>
       </c>
       <c r="B404" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C404" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="D404" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
@@ -8319,13 +8337,13 @@
         <v>287</v>
       </c>
       <c r="B405" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="C405" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D405" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -8333,13 +8351,13 @@
         <v>287</v>
       </c>
       <c r="B406" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C406" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D406" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -8347,69 +8365,69 @@
         <v>287</v>
       </c>
       <c r="B407" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="C407" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="D407" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B408" t="s">
         <v>21</v>
       </c>
       <c r="C408" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="D408" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B409" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C409" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D409" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B410" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C410" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D410" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B411" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C411" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="D411" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>